<commit_message>
Enhance data loading and processing in `erection_compiled_to_daily_new.py`
- Introduced robust error handling and fallback mechanisms for loading Excel sheets, improving reliability.
- Added functions to scrub defined names from Excel workbooks and export sheets via Excel COM, enhancing data integrity.
- Refactored header normalization and introduced canonical header key generation for better data consistency.
- Updated logging to provide clearer insights during the execution of the data processing pipeline.
- Made minor adjustments to the layout and styling in the dashboard for improved user experience.
</commit_message>
<xml_diff>
--- a/Raw Data/Micro Plans/Micro Plan TA-505 Oct '25.xlsx
+++ b/Raw Data/Micro Plans/Micro Plan TA-505 Oct '25.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaushikb\Documents\Work\Git\Office-work-\Raw Data\Micro Plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DFB8128-1BA9-4D0C-9015-643C31D9F0E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0BC03E-45DE-4FD2-B71D-DB72506C6A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1993,6 +1993,48 @@
     <xf numFmtId="166" fontId="11" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="9" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="9" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2012,6 +2054,66 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2032,18 +2134,6 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2053,55 +2143,28 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2115,69 +2178,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="9" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="9" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -2192,7 +2192,37 @@
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
     <cellStyle name="Percent 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
   </cellStyles>
-  <dxfs count="39">
+  <dxfs count="42">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2880,26 +2910,26 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="197" t="s">
+      <c r="A2" s="211" t="s">
         <v>116</v>
       </c>
-      <c r="B2" s="198"/>
-      <c r="C2" s="198"/>
-      <c r="D2" s="198"/>
-      <c r="E2" s="198"/>
-      <c r="F2" s="198"/>
-      <c r="G2" s="199"/>
+      <c r="B2" s="212"/>
+      <c r="C2" s="212"/>
+      <c r="D2" s="212"/>
+      <c r="E2" s="212"/>
+      <c r="F2" s="212"/>
+      <c r="G2" s="213"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="200" t="s">
+      <c r="A3" s="214" t="s">
         <v>196</v>
       </c>
-      <c r="B3" s="201"/>
-      <c r="C3" s="201"/>
-      <c r="D3" s="201"/>
-      <c r="E3" s="201"/>
-      <c r="F3" s="201"/>
-      <c r="G3" s="202"/>
+      <c r="B3" s="215"/>
+      <c r="C3" s="215"/>
+      <c r="D3" s="215"/>
+      <c r="E3" s="215"/>
+      <c r="F3" s="215"/>
+      <c r="G3" s="216"/>
     </row>
     <row r="4" spans="1:11" s="49" customFormat="1" ht="41.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="75" t="s">
@@ -2999,12 +3029,12 @@
     </row>
     <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="78"/>
-      <c r="B8" s="196" t="s">
+      <c r="B8" s="210" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="196"/>
-      <c r="D8" s="196"/>
-      <c r="E8" s="196"/>
+      <c r="C8" s="210"/>
+      <c r="D8" s="210"/>
+      <c r="E8" s="210"/>
       <c r="F8" s="79">
         <f>SUM(F5:F7)</f>
         <v>48075445.063227482</v>
@@ -3065,10 +3095,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="230" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="230"/>
+      <c r="A1" s="220" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="220"/>
       <c r="D1" s="17" t="s">
         <v>41</v>
       </c>
@@ -3155,24 +3185,24 @@
         <f>R51</f>
         <v>20193024.083227497</v>
       </c>
-      <c r="H9" s="231" t="s">
+      <c r="H9" s="221" t="s">
         <v>18</v>
       </c>
-      <c r="I9" s="231"/>
-      <c r="J9" s="231"/>
-      <c r="L9" s="227" t="s">
+      <c r="I9" s="221"/>
+      <c r="J9" s="221"/>
+      <c r="L9" s="217" t="s">
         <v>46</v>
       </c>
-      <c r="M9" s="227"/>
+      <c r="M9" s="217"/>
       <c r="N9" s="33">
         <f>E9*10539</f>
         <v>316170</v>
       </c>
-      <c r="O9" s="228">
+      <c r="O9" s="218">
         <f>G9+N9</f>
         <v>20509194.083227497</v>
       </c>
-      <c r="P9" s="229"/>
+      <c r="P9" s="219"/>
     </row>
     <row r="10" spans="1:16" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="7"/>
@@ -3304,8 +3334,8 @@
       </c>
       <c r="I15" s="40"/>
       <c r="J15" s="39"/>
-      <c r="O15" s="230"/>
-      <c r="P15" s="230"/>
+      <c r="O15" s="220"/>
+      <c r="P15" s="220"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
@@ -3332,19 +3362,19 @@
       </c>
       <c r="I16" s="41"/>
       <c r="J16" s="23"/>
-      <c r="L16" s="227" t="s">
+      <c r="L16" s="217" t="s">
         <v>45</v>
       </c>
-      <c r="M16" s="227"/>
+      <c r="M16" s="217"/>
       <c r="N16" s="33">
         <f>E16*10539</f>
         <v>10539</v>
       </c>
-      <c r="O16" s="228">
+      <c r="O16" s="218">
         <f>G16+N16</f>
         <v>574580.6</v>
       </c>
-      <c r="P16" s="229"/>
+      <c r="P16" s="219"/>
     </row>
     <row r="17" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="5"/>
@@ -3353,152 +3383,152 @@
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:37" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="216" t="s">
+      <c r="A18" s="224" t="s">
         <v>81</v>
       </c>
-      <c r="B18" s="218" t="s">
+      <c r="B18" s="226" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="211" t="s">
+      <c r="C18" s="229" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="218" t="s">
+      <c r="D18" s="226" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="211" t="s">
+      <c r="E18" s="229" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="211" t="s">
+      <c r="F18" s="229" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="211" t="s">
+      <c r="G18" s="229" t="s">
         <v>44</v>
       </c>
-      <c r="H18" s="211" t="s">
+      <c r="H18" s="229" t="s">
         <v>43</v>
       </c>
-      <c r="I18" s="211" t="s">
+      <c r="I18" s="229" t="s">
         <v>62</v>
       </c>
-      <c r="J18" s="223" t="s">
+      <c r="J18" s="233" t="s">
         <v>16</v>
       </c>
-      <c r="K18" s="223"/>
-      <c r="L18" s="223"/>
-      <c r="M18" s="223"/>
-      <c r="N18" s="223"/>
-      <c r="O18" s="223"/>
-      <c r="P18" s="223"/>
-      <c r="Q18" s="223"/>
-      <c r="R18" s="205" t="s">
+      <c r="K18" s="233"/>
+      <c r="L18" s="233"/>
+      <c r="M18" s="233"/>
+      <c r="N18" s="233"/>
+      <c r="O18" s="233"/>
+      <c r="P18" s="233"/>
+      <c r="Q18" s="233"/>
+      <c r="R18" s="239" t="s">
         <v>17</v>
       </c>
-      <c r="S18" s="203"/>
-      <c r="T18" s="211" t="s">
+      <c r="S18" s="237"/>
+      <c r="T18" s="229" t="s">
         <v>33</v>
       </c>
-      <c r="U18" s="203"/>
-      <c r="V18" s="213" t="s">
+      <c r="U18" s="237"/>
+      <c r="V18" s="243" t="s">
         <v>29</v>
       </c>
-      <c r="W18" s="214"/>
-      <c r="X18" s="214"/>
-      <c r="Y18" s="214"/>
-      <c r="Z18" s="214"/>
-      <c r="AA18" s="215"/>
+      <c r="W18" s="244"/>
+      <c r="X18" s="244"/>
+      <c r="Y18" s="244"/>
+      <c r="Z18" s="244"/>
+      <c r="AA18" s="245"/>
       <c r="AB18" s="71"/>
-      <c r="AC18" s="213" t="s">
+      <c r="AC18" s="243" t="s">
         <v>28</v>
       </c>
-      <c r="AD18" s="214"/>
-      <c r="AE18" s="214"/>
-      <c r="AF18" s="214"/>
-      <c r="AG18" s="214"/>
-      <c r="AH18" s="215"/>
-      <c r="AI18" s="207" t="s">
+      <c r="AD18" s="244"/>
+      <c r="AE18" s="244"/>
+      <c r="AF18" s="244"/>
+      <c r="AG18" s="244"/>
+      <c r="AH18" s="245"/>
+      <c r="AI18" s="241" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:37" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="217"/>
-      <c r="B19" s="219"/>
-      <c r="C19" s="221"/>
-      <c r="D19" s="219"/>
-      <c r="E19" s="221"/>
-      <c r="F19" s="221"/>
-      <c r="G19" s="221"/>
-      <c r="H19" s="221"/>
-      <c r="I19" s="221"/>
-      <c r="J19" s="224" t="s">
+      <c r="A19" s="225"/>
+      <c r="B19" s="227"/>
+      <c r="C19" s="230"/>
+      <c r="D19" s="227"/>
+      <c r="E19" s="230"/>
+      <c r="F19" s="230"/>
+      <c r="G19" s="230"/>
+      <c r="H19" s="230"/>
+      <c r="I19" s="230"/>
+      <c r="J19" s="234" t="s">
         <v>7</v>
       </c>
-      <c r="K19" s="224"/>
-      <c r="L19" s="224" t="s">
+      <c r="K19" s="234"/>
+      <c r="L19" s="234" t="s">
         <v>10</v>
       </c>
-      <c r="M19" s="224"/>
-      <c r="N19" s="224" t="s">
+      <c r="M19" s="234"/>
+      <c r="N19" s="234" t="s">
         <v>11</v>
       </c>
-      <c r="O19" s="224"/>
-      <c r="P19" s="225" t="s">
+      <c r="O19" s="234"/>
+      <c r="P19" s="235" t="s">
         <v>13</v>
       </c>
-      <c r="Q19" s="225" t="s">
+      <c r="Q19" s="235" t="s">
         <v>12</v>
       </c>
-      <c r="R19" s="206"/>
-      <c r="S19" s="204"/>
-      <c r="T19" s="212"/>
-      <c r="U19" s="204"/>
-      <c r="V19" s="209" t="s">
+      <c r="R19" s="240"/>
+      <c r="S19" s="238"/>
+      <c r="T19" s="232"/>
+      <c r="U19" s="238"/>
+      <c r="V19" s="222" t="s">
         <v>22</v>
       </c>
-      <c r="W19" s="209" t="s">
+      <c r="W19" s="222" t="s">
         <v>23</v>
       </c>
-      <c r="X19" s="209" t="s">
+      <c r="X19" s="222" t="s">
         <v>24</v>
       </c>
-      <c r="Y19" s="209" t="s">
+      <c r="Y19" s="222" t="s">
         <v>25</v>
       </c>
-      <c r="Z19" s="209" t="s">
+      <c r="Z19" s="222" t="s">
         <v>26</v>
       </c>
       <c r="AA19" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="AC19" s="209" t="s">
+      <c r="AC19" s="222" t="s">
         <v>22</v>
       </c>
-      <c r="AD19" s="209" t="s">
+      <c r="AD19" s="222" t="s">
         <v>23</v>
       </c>
-      <c r="AE19" s="209" t="s">
+      <c r="AE19" s="222" t="s">
         <v>24</v>
       </c>
-      <c r="AF19" s="209" t="s">
+      <c r="AF19" s="222" t="s">
         <v>25</v>
       </c>
-      <c r="AG19" s="209" t="s">
+      <c r="AG19" s="222" t="s">
         <v>26</v>
       </c>
       <c r="AH19" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="AI19" s="208"/>
+      <c r="AI19" s="242"/>
     </row>
     <row r="20" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="217"/>
-      <c r="B20" s="220"/>
-      <c r="C20" s="222"/>
-      <c r="D20" s="219"/>
-      <c r="E20" s="221"/>
-      <c r="F20" s="221"/>
-      <c r="G20" s="221"/>
-      <c r="H20" s="221"/>
-      <c r="I20" s="212"/>
+      <c r="A20" s="225"/>
+      <c r="B20" s="228"/>
+      <c r="C20" s="231"/>
+      <c r="D20" s="227"/>
+      <c r="E20" s="230"/>
+      <c r="F20" s="230"/>
+      <c r="G20" s="230"/>
+      <c r="H20" s="230"/>
+      <c r="I20" s="232"/>
       <c r="J20" s="34" t="s">
         <v>8</v>
       </c>
@@ -3517,25 +3547,25 @@
       <c r="O20" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="P20" s="226"/>
-      <c r="Q20" s="226"/>
+      <c r="P20" s="236"/>
+      <c r="Q20" s="236"/>
       <c r="R20" s="21" t="s">
         <v>37</v>
       </c>
       <c r="T20" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="V20" s="210"/>
-      <c r="W20" s="210"/>
-      <c r="X20" s="210"/>
-      <c r="Y20" s="210"/>
-      <c r="Z20" s="210"/>
+      <c r="V20" s="223"/>
+      <c r="W20" s="223"/>
+      <c r="X20" s="223"/>
+      <c r="Y20" s="223"/>
+      <c r="Z20" s="223"/>
       <c r="AA20" s="21"/>
-      <c r="AC20" s="210"/>
-      <c r="AD20" s="210"/>
-      <c r="AE20" s="210"/>
-      <c r="AF20" s="210"/>
-      <c r="AG20" s="210"/>
+      <c r="AC20" s="223"/>
+      <c r="AD20" s="223"/>
+      <c r="AE20" s="223"/>
+      <c r="AF20" s="223"/>
+      <c r="AG20" s="223"/>
       <c r="AH20" s="21" t="s">
         <v>37</v>
       </c>
@@ -6757,13 +6787,22 @@
   </sheetData>
   <autoFilter ref="A20:AI51" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="39">
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="S18:S19"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="AI18:AI19"/>
+    <mergeCell ref="AD19:AD20"/>
+    <mergeCell ref="AE19:AE20"/>
+    <mergeCell ref="AF19:AF20"/>
+    <mergeCell ref="AG19:AG20"/>
+    <mergeCell ref="T18:T19"/>
+    <mergeCell ref="U18:U19"/>
+    <mergeCell ref="V18:AA18"/>
+    <mergeCell ref="AC18:AH18"/>
+    <mergeCell ref="V19:V20"/>
+    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="X19:X20"/>
+    <mergeCell ref="Y19:Y20"/>
+    <mergeCell ref="Z19:Z20"/>
     <mergeCell ref="AC19:AC20"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="B18:B20"/>
@@ -6780,108 +6819,99 @@
     <mergeCell ref="N19:O19"/>
     <mergeCell ref="P19:P20"/>
     <mergeCell ref="Q19:Q20"/>
-    <mergeCell ref="S18:S19"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="AI18:AI19"/>
-    <mergeCell ref="AD19:AD20"/>
-    <mergeCell ref="AE19:AE20"/>
-    <mergeCell ref="AF19:AF20"/>
-    <mergeCell ref="AG19:AG20"/>
-    <mergeCell ref="T18:T19"/>
-    <mergeCell ref="U18:U19"/>
-    <mergeCell ref="V18:AA18"/>
-    <mergeCell ref="AC18:AH18"/>
-    <mergeCell ref="V19:V20"/>
-    <mergeCell ref="W19:W20"/>
-    <mergeCell ref="X19:X20"/>
-    <mergeCell ref="Y19:Y20"/>
-    <mergeCell ref="Z19:Z20"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="O15:P15"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B2:B20 B44:B1048576">
-    <cfRule type="duplicateValues" dxfId="38" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="37" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23 B21 B30:B33">
-    <cfRule type="duplicateValues" dxfId="36" priority="13090"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="13090"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:B29">
-    <cfRule type="duplicateValues" dxfId="35" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31:B40">
-    <cfRule type="duplicateValues" dxfId="34" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41">
-    <cfRule type="duplicateValues" dxfId="33" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="32" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42:B43">
-    <cfRule type="duplicateValues" dxfId="31" priority="23"/>
-    <cfRule type="duplicateValues" dxfId="30" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44:B50">
-    <cfRule type="duplicateValues" dxfId="29" priority="12992"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="12992"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B51:B1048576 B2:B20">
-    <cfRule type="duplicateValues" dxfId="28" priority="13"/>
-    <cfRule type="duplicateValues" dxfId="27" priority="14"/>
-    <cfRule type="duplicateValues" dxfId="26" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B51:B1048576">
-    <cfRule type="duplicateValues" dxfId="25" priority="16"/>
-    <cfRule type="duplicateValues" dxfId="24" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4">
-    <cfRule type="expression" dxfId="23" priority="13115" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="13115" stopIfTrue="1">
       <formula>AND(COUNTIF($C$173:$C$65319, N4)+COUNTIF($C$153:$C$154, N4)+COUNTIF($C$115:$C$116, N4)+COUNTIF($C$73:$C$76, N4)+COUNTIF(#REF!, N4)+COUNTIF(#REF!, N4)+COUNTIF(#REF!, N4)+COUNTIF(#REF!, N4)+COUNTIF(#REF!, N4)+COUNTIF(#REF!, N4)+COUNTIF(#REF!, N4)+COUNTIF($C$51:$C$52, N4)+COUNTIF(#REF!, N4)+COUNTIF($C$1:$C$20, N4)&gt;1,NOT(ISBLANK(N4)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="13116" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="13116" stopIfTrue="1">
       <formula>AND(COUNTIF($C$1:$C$65319, N4)+COUNTIF(#REF!, N4)&gt;1,NOT(ISBLANK(N4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4">
-    <cfRule type="expression" dxfId="21" priority="13117" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="13117" stopIfTrue="1">
       <formula>AND(COUNTIF($D$190:$D$65319, O4)+COUNTIF($D$1:$D$20, O4)+COUNTIF(#REF!, O4)+COUNTIF($D$173:$D$174, O4)+COUNTIF($D$153:$D$154, O4)+COUNTIF($D$115:$D$116, O4)+COUNTIF($D$73:$D$76, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)&gt;1,NOT(ISBLANK(O4)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="13118" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="13118" stopIfTrue="1">
       <formula>AND(COUNTIF($D$173:$D$65319, O4)+COUNTIF(#REF!, O4)+COUNTIF($D$1:$D$20, O4)+COUNTIF($D$153:$D$154, O4)+COUNTIF($D$115:$D$116, O4)+COUNTIF($D$73:$D$76, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)&gt;1,NOT(ISBLANK(O4)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="13119" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="13119" stopIfTrue="1">
       <formula>AND(COUNTIF($D$153:$D$65319, O4)+COUNTIF($D$1:$D$20, O4)+COUNTIF($D$115:$D$116, O4)+COUNTIF(#REF!, O4)+COUNTIF($D$73:$D$76, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)&gt;1,NOT(ISBLANK(O4)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="13120" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="13120" stopIfTrue="1">
       <formula>AND(COUNTIF($D$115:$D$65319, O4)+COUNTIF($D$1:$D$20, O4)+COUNTIF(#REF!, O4)+COUNTIF($D$73:$D$76, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)&gt;1,NOT(ISBLANK(O4)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="13121" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="13121" stopIfTrue="1">
       <formula>AND(COUNTIF($D$73:$D$65319, O4)+COUNTIF(#REF!, O4)+COUNTIF($D$1:$D$20, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)&gt;1,NOT(ISBLANK(O4)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="13122" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="13122" stopIfTrue="1">
       <formula>AND(COUNTIF($D$73:$D$65319, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF($D$1:$D$20, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)&gt;1,NOT(ISBLANK(O4)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="13123" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="13123" stopIfTrue="1">
       <formula>AND(COUNTIF($D$54:$D$65319, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF($D$1:$D$20, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)&gt;1,NOT(ISBLANK(O4)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="13124" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="13124" stopIfTrue="1">
       <formula>AND(COUNTIF($F$228:$F$65313, O4)+COUNTIF($F$1:$F$20, O4)+COUNTIF(#REF!, O4)+COUNTIF($F$211:$F$212, O4)+COUNTIF($F$191:$F$192, O4)+COUNTIF($F$153:$F$154, O4)+COUNTIF($F$111:$F$114, O4)+COUNTIF($F$88:$F$89, O4)+COUNTIF($F$61:$F$62, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)&gt;1,NOT(ISBLANK(O4)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="13125" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="13125" stopIfTrue="1">
       <formula>AND(COUNTIF($F$211:$F$65313, O4)+COUNTIF(#REF!, O4)+COUNTIF($F$1:$F$20, O4)+COUNTIF($F$191:$F$192, O4)+COUNTIF($F$153:$F$154, O4)+COUNTIF($F$111:$F$114, O4)+COUNTIF($F$88:$F$89, O4)+COUNTIF($F$61:$F$62, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)&gt;1,NOT(ISBLANK(O4)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="13126" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="13126" stopIfTrue="1">
       <formula>AND(COUNTIF($F$191:$F$65313, O4)+COUNTIF($F$1:$F$20, O4)+COUNTIF($F$153:$F$154, O4)+COUNTIF(#REF!, O4)+COUNTIF($F$111:$F$114, O4)+COUNTIF($F$88:$F$89, O4)+COUNTIF($F$61:$F$62, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)&gt;1,NOT(ISBLANK(O4)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="13127" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="13127" stopIfTrue="1">
       <formula>AND(COUNTIF($F$153:$F$65313, O4)+COUNTIF($F$1:$F$20, O4)+COUNTIF(#REF!, O4)+COUNTIF($F$111:$F$114, O4)+COUNTIF($F$88:$F$89, O4)+COUNTIF($F$61:$F$62, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)&gt;1,NOT(ISBLANK(O4)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="13128" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="13128" stopIfTrue="1">
       <formula>AND(COUNTIF($F$111:$F$65313, O4)+COUNTIF(#REF!, O4)+COUNTIF($F$1:$F$20, O4)+COUNTIF($F$88:$F$89, O4)+COUNTIF($F$61:$F$62, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)&gt;1,NOT(ISBLANK(O4)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="13129" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="13129" stopIfTrue="1">
       <formula>AND(COUNTIF($F$111:$F$65313, O4)+COUNTIF($F$88:$F$89, O4)+COUNTIF($F$61:$F$62, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF($F$1:$F$20, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)&gt;1,NOT(ISBLANK(O4)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="13130" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="13130" stopIfTrue="1">
       <formula>AND(COUNTIF($F$88:$F$65313, O4)+COUNTIF($F$61:$F$62, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF($F$1:$F$20, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)+COUNTIF(#REF!, O4)&gt;1,NOT(ISBLANK(O4)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6898,8 +6928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B32678F0-2B5B-4A2D-A796-1BCE3C3C0190}">
   <dimension ref="A1:AH74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="77" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView tabSelected="1" topLeftCell="E59" zoomScale="76" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="M67" sqref="M67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7167,128 +7197,128 @@
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:34" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="250"/>
-      <c r="B18" s="252"/>
-      <c r="C18" s="252"/>
-      <c r="D18" s="252"/>
-      <c r="E18" s="255"/>
-      <c r="F18" s="223" t="s">
+      <c r="A18" s="202"/>
+      <c r="B18" s="204"/>
+      <c r="C18" s="204"/>
+      <c r="D18" s="204"/>
+      <c r="E18" s="207"/>
+      <c r="F18" s="233" t="s">
         <v>16</v>
       </c>
-      <c r="G18" s="223"/>
-      <c r="H18" s="223"/>
-      <c r="I18" s="223"/>
-      <c r="J18" s="223"/>
+      <c r="G18" s="233"/>
+      <c r="H18" s="233"/>
+      <c r="I18" s="233"/>
+      <c r="J18" s="233"/>
       <c r="K18" s="65"/>
       <c r="L18" s="137"/>
       <c r="M18" s="137"/>
       <c r="N18" s="137"/>
       <c r="O18" s="137"/>
       <c r="P18" s="137"/>
-      <c r="Q18" s="233"/>
+      <c r="Q18" s="254"/>
       <c r="R18" s="144"/>
-      <c r="S18" s="235" t="s">
+      <c r="S18" s="256" t="s">
         <v>33</v>
       </c>
       <c r="T18" s="71"/>
-      <c r="U18" s="237" t="s">
+      <c r="U18" s="251" t="s">
         <v>29</v>
       </c>
-      <c r="V18" s="238"/>
-      <c r="W18" s="238"/>
-      <c r="X18" s="238"/>
-      <c r="Y18" s="238"/>
-      <c r="Z18" s="239"/>
+      <c r="V18" s="252"/>
+      <c r="W18" s="252"/>
+      <c r="X18" s="252"/>
+      <c r="Y18" s="252"/>
+      <c r="Z18" s="253"/>
       <c r="AA18" s="71"/>
-      <c r="AB18" s="237" t="s">
+      <c r="AB18" s="251" t="s">
         <v>28</v>
       </c>
-      <c r="AC18" s="238"/>
-      <c r="AD18" s="238"/>
-      <c r="AE18" s="238"/>
-      <c r="AF18" s="238"/>
-      <c r="AG18" s="239"/>
-      <c r="AH18" s="240" t="s">
+      <c r="AC18" s="252"/>
+      <c r="AD18" s="252"/>
+      <c r="AE18" s="252"/>
+      <c r="AF18" s="252"/>
+      <c r="AG18" s="253"/>
+      <c r="AH18" s="248" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:34" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="251"/>
-      <c r="B19" s="253"/>
-      <c r="C19" s="253"/>
-      <c r="D19" s="254"/>
-      <c r="E19" s="254"/>
-      <c r="F19" s="256"/>
-      <c r="G19" s="242" t="s">
+      <c r="A19" s="203"/>
+      <c r="B19" s="205"/>
+      <c r="C19" s="205"/>
+      <c r="D19" s="206"/>
+      <c r="E19" s="206"/>
+      <c r="F19" s="208"/>
+      <c r="G19" s="246" t="s">
         <v>47</v>
       </c>
-      <c r="H19" s="243"/>
-      <c r="I19" s="256"/>
-      <c r="J19" s="256"/>
-      <c r="K19" s="257"/>
-      <c r="L19" s="257"/>
-      <c r="M19" s="244"/>
-      <c r="N19" s="244"/>
-      <c r="O19" s="244"/>
-      <c r="P19" s="244"/>
-      <c r="Q19" s="234"/>
+      <c r="H19" s="247"/>
+      <c r="I19" s="208"/>
+      <c r="J19" s="208"/>
+      <c r="K19" s="209"/>
+      <c r="L19" s="209"/>
+      <c r="M19" s="196"/>
+      <c r="N19" s="196"/>
+      <c r="O19" s="196"/>
+      <c r="P19" s="196"/>
+      <c r="Q19" s="255"/>
       <c r="R19" s="145"/>
-      <c r="S19" s="236"/>
-      <c r="U19" s="232" t="s">
+      <c r="S19" s="257"/>
+      <c r="U19" s="250" t="s">
         <v>22</v>
       </c>
-      <c r="V19" s="232" t="s">
+      <c r="V19" s="250" t="s">
         <v>23</v>
       </c>
-      <c r="W19" s="232" t="s">
+      <c r="W19" s="250" t="s">
         <v>24</v>
       </c>
-      <c r="X19" s="232" t="s">
+      <c r="X19" s="250" t="s">
         <v>25</v>
       </c>
-      <c r="Y19" s="232" t="s">
+      <c r="Y19" s="250" t="s">
         <v>26</v>
       </c>
       <c r="Z19" s="140" t="s">
         <v>27</v>
       </c>
-      <c r="AB19" s="232" t="s">
+      <c r="AB19" s="250" t="s">
         <v>22</v>
       </c>
-      <c r="AC19" s="232" t="s">
+      <c r="AC19" s="250" t="s">
         <v>23</v>
       </c>
-      <c r="AD19" s="232" t="s">
+      <c r="AD19" s="250" t="s">
         <v>24</v>
       </c>
-      <c r="AE19" s="232" t="s">
+      <c r="AE19" s="250" t="s">
         <v>25</v>
       </c>
-      <c r="AF19" s="232" t="s">
+      <c r="AF19" s="250" t="s">
         <v>26</v>
       </c>
       <c r="AG19" s="140" t="s">
         <v>207</v>
       </c>
-      <c r="AH19" s="241"/>
+      <c r="AH19" s="249"/>
     </row>
     <row r="20" spans="1:34" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="250" t="s">
+      <c r="A20" s="202" t="s">
         <v>81</v>
       </c>
-      <c r="B20" s="252" t="s">
+      <c r="B20" s="204" t="s">
         <v>198</v>
       </c>
-      <c r="C20" s="252" t="s">
+      <c r="C20" s="204" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="252" t="s">
+      <c r="D20" s="204" t="s">
         <v>199</v>
       </c>
-      <c r="E20" s="255" t="s">
+      <c r="E20" s="207" t="s">
         <v>200</v>
       </c>
-      <c r="F20" s="256" t="s">
+      <c r="F20" s="208" t="s">
         <v>203</v>
       </c>
       <c r="G20" s="34" t="s">
@@ -7297,28 +7327,28 @@
       <c r="H20" s="34" t="s">
         <v>202</v>
       </c>
-      <c r="I20" s="256" t="s">
+      <c r="I20" s="208" t="s">
         <v>49</v>
       </c>
-      <c r="J20" s="256" t="s">
+      <c r="J20" s="208" t="s">
         <v>50</v>
       </c>
-      <c r="K20" s="257" t="s">
+      <c r="K20" s="209" t="s">
         <v>66</v>
       </c>
-      <c r="L20" s="257" t="s">
+      <c r="L20" s="209" t="s">
         <v>204</v>
       </c>
-      <c r="M20" s="245" t="s">
+      <c r="M20" s="197" t="s">
         <v>212</v>
       </c>
-      <c r="N20" s="245" t="s">
+      <c r="N20" s="197" t="s">
         <v>207</v>
       </c>
-      <c r="O20" s="245" t="s">
+      <c r="O20" s="197" t="s">
         <v>213</v>
       </c>
-      <c r="P20" s="245" t="s">
+      <c r="P20" s="197" t="s">
         <v>214</v>
       </c>
       <c r="Q20" s="118" t="s">
@@ -7328,17 +7358,17 @@
       <c r="S20" s="141" t="s">
         <v>34</v>
       </c>
-      <c r="U20" s="220"/>
-      <c r="V20" s="220"/>
-      <c r="W20" s="220"/>
-      <c r="X20" s="220"/>
-      <c r="Y20" s="220"/>
+      <c r="U20" s="228"/>
+      <c r="V20" s="228"/>
+      <c r="W20" s="228"/>
+      <c r="X20" s="228"/>
+      <c r="Y20" s="228"/>
       <c r="Z20" s="119"/>
-      <c r="AB20" s="220"/>
-      <c r="AC20" s="220"/>
-      <c r="AD20" s="220"/>
-      <c r="AE20" s="220"/>
-      <c r="AF20" s="220"/>
+      <c r="AB20" s="228"/>
+      <c r="AC20" s="228"/>
+      <c r="AD20" s="228"/>
+      <c r="AE20" s="228"/>
+      <c r="AF20" s="228"/>
       <c r="AG20" s="119" t="s">
         <v>18</v>
       </c>
@@ -7374,7 +7404,7 @@
         <v>45938</v>
       </c>
       <c r="I21" s="110">
-        <f t="shared" ref="I21:I24" si="2">H21+1</f>
+        <f t="shared" ref="I21:J36" si="2">H21+1</f>
         <v>45939</v>
       </c>
       <c r="J21" s="110">
@@ -7392,7 +7422,6 @@
       <c r="O21" s="111"/>
       <c r="P21" s="111"/>
       <c r="Q21" s="112">
-        <f>D21*10940</f>
         <v>773950.3</v>
       </c>
       <c r="R21" s="145"/>
@@ -7484,7 +7513,6 @@
       <c r="O22" s="111"/>
       <c r="P22" s="111"/>
       <c r="Q22" s="112">
-        <f>D22*10940</f>
         <v>499925.18000000005</v>
       </c>
       <c r="R22" s="145"/>
@@ -7562,7 +7590,7 @@
         <v>45953</v>
       </c>
       <c r="J23" s="110">
-        <f t="shared" ref="J23:J24" si="12">I23+1</f>
+        <f t="shared" si="2"/>
         <v>45954</v>
       </c>
       <c r="K23" s="111" t="s">
@@ -7576,7 +7604,6 @@
       <c r="O23" s="111"/>
       <c r="P23" s="111"/>
       <c r="Q23" s="112">
-        <f t="shared" ref="Q23:Q26" si="13">D23*10940</f>
         <v>683137.36</v>
       </c>
       <c r="R23" s="145"/>
@@ -7654,7 +7681,7 @@
         <v>45960</v>
       </c>
       <c r="J24" s="110">
-        <f t="shared" si="12"/>
+        <f t="shared" si="2"/>
         <v>45961</v>
       </c>
       <c r="K24" s="111" t="s">
@@ -7668,7 +7695,6 @@
       <c r="O24" s="111"/>
       <c r="P24" s="111"/>
       <c r="Q24" s="112">
-        <f t="shared" si="13"/>
         <v>720650.62</v>
       </c>
       <c r="R24" s="145"/>
@@ -7737,11 +7763,11 @@
         <v>45932</v>
       </c>
       <c r="H25" s="110">
-        <f t="shared" ref="H25:H30" si="14">G25+8</f>
+        <f t="shared" ref="H25:H30" si="12">G25+8</f>
         <v>45940</v>
       </c>
       <c r="I25" s="110">
-        <f t="shared" ref="I25:I27" si="15">H25+1</f>
+        <f t="shared" si="2"/>
         <v>45941</v>
       </c>
       <c r="J25" s="110">
@@ -7759,7 +7785,6 @@
       <c r="O25" s="111"/>
       <c r="P25" s="111"/>
       <c r="Q25" s="112">
-        <f t="shared" si="13"/>
         <v>843222.38</v>
       </c>
       <c r="R25" s="145"/>
@@ -7825,15 +7850,15 @@
         <v>45940</v>
       </c>
       <c r="G26" s="110">
-        <f t="shared" ref="G26" si="16">H25+1</f>
+        <f t="shared" ref="G26" si="13">H25+1</f>
         <v>45941</v>
       </c>
       <c r="H26" s="110">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>45949</v>
       </c>
       <c r="I26" s="110">
-        <f t="shared" si="15"/>
+        <f t="shared" si="2"/>
         <v>45950</v>
       </c>
       <c r="J26" s="110">
@@ -7851,7 +7876,6 @@
       <c r="O26" s="111"/>
       <c r="P26" s="111"/>
       <c r="Q26" s="112">
-        <f t="shared" si="13"/>
         <v>773950.3</v>
       </c>
       <c r="R26" s="145"/>
@@ -7921,15 +7945,15 @@
         <v>45950</v>
       </c>
       <c r="H27" s="110">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>45958</v>
       </c>
       <c r="I27" s="110">
-        <f t="shared" si="15"/>
+        <f t="shared" si="2"/>
         <v>45959</v>
       </c>
       <c r="J27" s="110">
-        <f t="shared" ref="J27" si="17">I27+1</f>
+        <f t="shared" si="2"/>
         <v>45960</v>
       </c>
       <c r="K27" s="111" t="s">
@@ -7943,7 +7967,6 @@
       <c r="O27" s="111"/>
       <c r="P27" s="111"/>
       <c r="Q27" s="112">
-        <f>D27*10940</f>
         <v>1063017.9200000002</v>
       </c>
       <c r="R27" s="145"/>
@@ -8012,11 +8035,11 @@
         <v>45932</v>
       </c>
       <c r="H28" s="110">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>45940</v>
       </c>
       <c r="I28" s="110">
-        <f t="shared" ref="I28:I30" si="18">H28+1</f>
+        <f t="shared" si="2"/>
         <v>45941</v>
       </c>
       <c r="J28" s="110">
@@ -8034,7 +8057,6 @@
       <c r="O28" s="111"/>
       <c r="P28" s="111"/>
       <c r="Q28" s="112">
-        <f>D28*10940</f>
         <v>395590.39999999997</v>
       </c>
       <c r="R28" s="145"/>
@@ -8100,15 +8122,15 @@
         <v>45940</v>
       </c>
       <c r="G29" s="110">
-        <f t="shared" ref="G29" si="19">H28+1</f>
+        <f t="shared" ref="G29" si="14">H28+1</f>
         <v>45941</v>
       </c>
       <c r="H29" s="110">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>45949</v>
       </c>
       <c r="I29" s="110">
-        <f t="shared" si="18"/>
+        <f t="shared" si="2"/>
         <v>45950</v>
       </c>
       <c r="J29" s="110">
@@ -8126,7 +8148,6 @@
       <c r="O29" s="111"/>
       <c r="P29" s="111"/>
       <c r="Q29" s="112">
-        <f>D29*10940</f>
         <v>414965.13999999996</v>
       </c>
       <c r="R29" s="145"/>
@@ -8196,15 +8217,15 @@
         <v>45950</v>
       </c>
       <c r="H30" s="110">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>45958</v>
       </c>
       <c r="I30" s="110">
-        <f t="shared" si="18"/>
+        <f t="shared" si="2"/>
         <v>45959</v>
       </c>
       <c r="J30" s="110">
-        <f t="shared" ref="J30" si="20">I30+1</f>
+        <f t="shared" si="2"/>
         <v>45960</v>
       </c>
       <c r="K30" s="111" t="s">
@@ -8218,7 +8239,6 @@
       <c r="O30" s="111"/>
       <c r="P30" s="111"/>
       <c r="Q30" s="112">
-        <f>D30*10940</f>
         <v>711406.32000000007</v>
       </c>
       <c r="R30" s="145"/>
@@ -8291,7 +8311,7 @@
         <v>45937</v>
       </c>
       <c r="I31" s="110">
-        <f t="shared" ref="I31:I34" si="21">H31+1</f>
+        <f t="shared" si="2"/>
         <v>45938</v>
       </c>
       <c r="J31" s="110">
@@ -8309,7 +8329,6 @@
       <c r="O31" s="111"/>
       <c r="P31" s="111"/>
       <c r="Q31" s="112">
-        <f t="shared" ref="Q31:Q46" si="22">D31*10940</f>
         <v>414965.13999999996</v>
       </c>
       <c r="R31" s="145"/>
@@ -8375,7 +8394,7 @@
         <v>45937</v>
       </c>
       <c r="G32" s="110">
-        <f t="shared" ref="G32" si="23">H31+1</f>
+        <f t="shared" ref="G32" si="15">H31+1</f>
         <v>45938</v>
       </c>
       <c r="H32" s="110">
@@ -8383,7 +8402,7 @@
         <v>45943</v>
       </c>
       <c r="I32" s="110">
-        <f t="shared" si="21"/>
+        <f t="shared" si="2"/>
         <v>45944</v>
       </c>
       <c r="J32" s="110">
@@ -8401,7 +8420,6 @@
       <c r="O32" s="111"/>
       <c r="P32" s="111"/>
       <c r="Q32" s="112">
-        <f t="shared" si="22"/>
         <v>801300.3</v>
       </c>
       <c r="R32" s="145"/>
@@ -8475,11 +8493,11 @@
         <v>45950</v>
       </c>
       <c r="I33" s="110">
-        <f t="shared" si="21"/>
+        <f t="shared" si="2"/>
         <v>45951</v>
       </c>
       <c r="J33" s="110">
-        <f t="shared" ref="J33:J34" si="24">I33+1</f>
+        <f t="shared" si="2"/>
         <v>45952</v>
       </c>
       <c r="K33" s="111" t="s">
@@ -8493,7 +8511,6 @@
       <c r="O33" s="111"/>
       <c r="P33" s="111"/>
       <c r="Q33" s="112">
-        <f t="shared" si="22"/>
         <v>389485.87999999995</v>
       </c>
       <c r="R33" s="145"/>
@@ -8567,11 +8584,11 @@
         <v>45959</v>
       </c>
       <c r="I34" s="110">
-        <f t="shared" si="21"/>
+        <f t="shared" si="2"/>
         <v>45960</v>
       </c>
       <c r="J34" s="110">
-        <f t="shared" si="24"/>
+        <f t="shared" si="2"/>
         <v>45961</v>
       </c>
       <c r="K34" s="111" t="s">
@@ -8585,7 +8602,6 @@
       <c r="O34" s="111"/>
       <c r="P34" s="111"/>
       <c r="Q34" s="112">
-        <f t="shared" si="22"/>
         <v>895209.25999999989</v>
       </c>
       <c r="R34" s="145"/>
@@ -8658,7 +8674,7 @@
         <v>45936</v>
       </c>
       <c r="I35" s="110">
-        <f t="shared" ref="I35:I41" si="25">H35+1</f>
+        <f t="shared" si="2"/>
         <v>45937</v>
       </c>
       <c r="J35" s="110">
@@ -8671,12 +8687,11 @@
       <c r="L35" s="111" t="s">
         <v>64</v>
       </c>
-      <c r="M35" s="246"/>
-      <c r="N35" s="246"/>
-      <c r="O35" s="246"/>
-      <c r="P35" s="246"/>
+      <c r="M35" s="198"/>
+      <c r="N35" s="198"/>
+      <c r="O35" s="198"/>
+      <c r="P35" s="198"/>
       <c r="Q35" s="117">
-        <f t="shared" si="22"/>
         <v>395590.39999999997</v>
       </c>
       <c r="R35" s="145"/>
@@ -8742,7 +8757,7 @@
         <v>45936</v>
       </c>
       <c r="G36" s="110">
-        <f t="shared" ref="G36" si="26">H35+1</f>
+        <f t="shared" ref="G36" si="16">H35+1</f>
         <v>45937</v>
       </c>
       <c r="H36" s="110">
@@ -8750,7 +8765,7 @@
         <v>45946</v>
       </c>
       <c r="I36" s="110">
-        <f t="shared" si="25"/>
+        <f t="shared" si="2"/>
         <v>45947</v>
       </c>
       <c r="J36" s="110">
@@ -8763,12 +8778,11 @@
       <c r="L36" s="111" t="s">
         <v>64</v>
       </c>
-      <c r="M36" s="246"/>
-      <c r="N36" s="246"/>
-      <c r="O36" s="246"/>
-      <c r="P36" s="246"/>
+      <c r="M36" s="198"/>
+      <c r="N36" s="198"/>
+      <c r="O36" s="198"/>
+      <c r="P36" s="198"/>
       <c r="Q36" s="117">
-        <f t="shared" si="22"/>
         <v>1063017.9200000002</v>
       </c>
       <c r="R36" s="145"/>
@@ -8842,11 +8856,11 @@
         <v>45959</v>
       </c>
       <c r="I37" s="110">
-        <f t="shared" si="25"/>
+        <f t="shared" ref="I37:J52" si="17">H37+1</f>
         <v>45960</v>
       </c>
       <c r="J37" s="110">
-        <f t="shared" ref="J37" si="27">I37+1</f>
+        <f t="shared" si="17"/>
         <v>45961</v>
       </c>
       <c r="K37" s="111" t="s">
@@ -8855,12 +8869,11 @@
       <c r="L37" s="111" t="s">
         <v>64</v>
       </c>
-      <c r="M37" s="246"/>
-      <c r="N37" s="246"/>
-      <c r="O37" s="246"/>
-      <c r="P37" s="246"/>
+      <c r="M37" s="198"/>
+      <c r="N37" s="198"/>
+      <c r="O37" s="198"/>
+      <c r="P37" s="198"/>
       <c r="Q37" s="117">
-        <f t="shared" si="22"/>
         <v>1366953</v>
       </c>
       <c r="R37" s="145"/>
@@ -8933,7 +8946,7 @@
         <v>45938</v>
       </c>
       <c r="I38" s="178">
-        <f t="shared" si="25"/>
+        <f t="shared" si="17"/>
         <v>45939</v>
       </c>
       <c r="J38" s="178">
@@ -8946,12 +8959,11 @@
       <c r="L38" s="179" t="s">
         <v>64</v>
       </c>
-      <c r="M38" s="247"/>
-      <c r="N38" s="247"/>
-      <c r="O38" s="247"/>
-      <c r="P38" s="247"/>
+      <c r="M38" s="199"/>
+      <c r="N38" s="199"/>
+      <c r="O38" s="199"/>
+      <c r="P38" s="199"/>
       <c r="Q38" s="180">
-        <f t="shared" si="22"/>
         <v>952009.74</v>
       </c>
       <c r="R38" s="181"/>
@@ -9021,7 +9033,7 @@
         <v>45938</v>
       </c>
       <c r="G39" s="110">
-        <f t="shared" ref="G39" si="28">H38+1</f>
+        <f t="shared" ref="G39" si="18">H38+1</f>
         <v>45939</v>
       </c>
       <c r="H39" s="110">
@@ -9029,7 +9041,7 @@
         <v>45947</v>
       </c>
       <c r="I39" s="110">
-        <f t="shared" si="25"/>
+        <f t="shared" si="17"/>
         <v>45948</v>
       </c>
       <c r="J39" s="110">
@@ -9042,12 +9054,11 @@
       <c r="L39" s="111" t="s">
         <v>64</v>
       </c>
-      <c r="M39" s="246"/>
-      <c r="N39" s="246"/>
-      <c r="O39" s="246"/>
-      <c r="P39" s="246"/>
+      <c r="M39" s="198"/>
+      <c r="N39" s="198"/>
+      <c r="O39" s="198"/>
+      <c r="P39" s="198"/>
       <c r="Q39" s="117">
-        <f t="shared" si="22"/>
         <v>735846.28</v>
       </c>
       <c r="R39" s="145"/>
@@ -9121,11 +9132,11 @@
         <v>45953</v>
       </c>
       <c r="I40" s="110">
-        <f t="shared" si="25"/>
+        <f t="shared" si="17"/>
         <v>45954</v>
       </c>
       <c r="J40" s="110">
-        <f t="shared" ref="J40:J41" si="29">I40+1</f>
+        <f t="shared" si="17"/>
         <v>45955</v>
       </c>
       <c r="K40" s="111" t="s">
@@ -9134,10 +9145,10 @@
       <c r="L40" s="111" t="s">
         <v>64</v>
       </c>
-      <c r="M40" s="246"/>
-      <c r="N40" s="246"/>
-      <c r="O40" s="246"/>
-      <c r="P40" s="246"/>
+      <c r="M40" s="198"/>
+      <c r="N40" s="198"/>
+      <c r="O40" s="198"/>
+      <c r="P40" s="198"/>
       <c r="Q40" s="117">
         <v>414965.13999999996</v>
       </c>
@@ -9212,11 +9223,11 @@
         <v>45959</v>
       </c>
       <c r="I41" s="110">
-        <f t="shared" si="25"/>
+        <f t="shared" si="17"/>
         <v>45960</v>
       </c>
       <c r="J41" s="110">
-        <f t="shared" si="29"/>
+        <f t="shared" si="17"/>
         <v>45961</v>
       </c>
       <c r="K41" s="111" t="s">
@@ -9225,10 +9236,10 @@
       <c r="L41" s="111" t="s">
         <v>64</v>
       </c>
-      <c r="M41" s="246"/>
-      <c r="N41" s="246"/>
-      <c r="O41" s="246"/>
-      <c r="P41" s="246"/>
+      <c r="M41" s="198"/>
+      <c r="N41" s="198"/>
+      <c r="O41" s="198"/>
+      <c r="P41" s="198"/>
       <c r="Q41" s="117">
         <v>414965.13999999996</v>
       </c>
@@ -9302,7 +9313,7 @@
         <v>45942</v>
       </c>
       <c r="I42" s="178">
-        <f t="shared" ref="I42:I44" si="30">H42+1</f>
+        <f t="shared" si="17"/>
         <v>45943</v>
       </c>
       <c r="J42" s="178">
@@ -9320,7 +9331,6 @@
       <c r="O42" s="179"/>
       <c r="P42" s="179"/>
       <c r="Q42" s="193">
-        <f t="shared" ref="Q42" si="31">D42*10940</f>
         <v>683137.36</v>
       </c>
       <c r="R42" s="181"/>
@@ -9390,7 +9400,7 @@
         <v>45942</v>
       </c>
       <c r="G43" s="110">
-        <f t="shared" ref="G43" si="32">H42+1</f>
+        <f t="shared" ref="G43" si="19">H42+1</f>
         <v>45943</v>
       </c>
       <c r="H43" s="110">
@@ -9398,7 +9408,7 @@
         <v>45953</v>
       </c>
       <c r="I43" s="110">
-        <f t="shared" si="30"/>
+        <f t="shared" si="17"/>
         <v>45954</v>
       </c>
       <c r="J43" s="110">
@@ -9411,10 +9421,10 @@
       <c r="L43" s="110" t="s">
         <v>206</v>
       </c>
-      <c r="M43" s="248"/>
-      <c r="N43" s="248"/>
-      <c r="O43" s="248"/>
-      <c r="P43" s="248"/>
+      <c r="M43" s="200"/>
+      <c r="N43" s="200"/>
+      <c r="O43" s="200"/>
+      <c r="P43" s="200"/>
       <c r="Q43" s="117">
         <v>823552.26</v>
       </c>
@@ -9485,15 +9495,15 @@
         <v>45954</v>
       </c>
       <c r="H44" s="110">
-        <f t="shared" ref="H44:H49" si="33">G44+5</f>
+        <f t="shared" ref="H44:H49" si="20">G44+5</f>
         <v>45959</v>
       </c>
       <c r="I44" s="110">
-        <f t="shared" si="30"/>
+        <f t="shared" si="17"/>
         <v>45960</v>
       </c>
       <c r="J44" s="110">
-        <f t="shared" ref="J44" si="34">I44+1</f>
+        <f t="shared" si="17"/>
         <v>45961</v>
       </c>
       <c r="K44" s="111" t="s">
@@ -9502,10 +9512,10 @@
       <c r="L44" s="110" t="s">
         <v>206</v>
       </c>
-      <c r="M44" s="248"/>
-      <c r="N44" s="248"/>
-      <c r="O44" s="248"/>
-      <c r="P44" s="248"/>
+      <c r="M44" s="200"/>
+      <c r="N44" s="200"/>
+      <c r="O44" s="200"/>
+      <c r="P44" s="200"/>
       <c r="Q44" s="117">
         <v>414965.13999999996</v>
       </c>
@@ -9575,11 +9585,11 @@
         <v>45932</v>
       </c>
       <c r="H45" s="110">
-        <f t="shared" si="33"/>
+        <f t="shared" si="20"/>
         <v>45937</v>
       </c>
       <c r="I45" s="110">
-        <f t="shared" ref="I45:I49" si="35">H45+1</f>
+        <f t="shared" si="17"/>
         <v>45938</v>
       </c>
       <c r="J45" s="110">
@@ -9592,12 +9602,11 @@
       <c r="L45" s="110" t="s">
         <v>206</v>
       </c>
-      <c r="M45" s="248"/>
-      <c r="N45" s="248"/>
-      <c r="O45" s="248"/>
-      <c r="P45" s="248"/>
+      <c r="M45" s="200"/>
+      <c r="N45" s="200"/>
+      <c r="O45" s="200"/>
+      <c r="P45" s="200"/>
       <c r="Q45" s="117">
-        <f t="shared" si="22"/>
         <v>414965.13999999996</v>
       </c>
       <c r="R45" s="145"/>
@@ -9663,15 +9672,15 @@
         <v>45937</v>
       </c>
       <c r="G46" s="110">
-        <f t="shared" ref="G46" si="36">H45+1</f>
+        <f t="shared" ref="G46" si="21">H45+1</f>
         <v>45938</v>
       </c>
       <c r="H46" s="110">
-        <f t="shared" si="33"/>
+        <f t="shared" si="20"/>
         <v>45943</v>
       </c>
       <c r="I46" s="110">
-        <f t="shared" si="35"/>
+        <f t="shared" si="17"/>
         <v>45944</v>
       </c>
       <c r="J46" s="110">
@@ -9684,12 +9693,11 @@
       <c r="L46" s="110" t="s">
         <v>206</v>
       </c>
-      <c r="M46" s="248"/>
-      <c r="N46" s="248"/>
-      <c r="O46" s="248"/>
-      <c r="P46" s="248"/>
+      <c r="M46" s="200"/>
+      <c r="N46" s="200"/>
+      <c r="O46" s="200"/>
+      <c r="P46" s="200"/>
       <c r="Q46" s="117">
-        <f t="shared" si="22"/>
         <v>499925.18000000005</v>
       </c>
       <c r="R46" s="145"/>
@@ -9759,15 +9767,15 @@
         <v>45944</v>
       </c>
       <c r="H47" s="110">
-        <f t="shared" si="33"/>
+        <f t="shared" si="20"/>
         <v>45949</v>
       </c>
       <c r="I47" s="110">
-        <f t="shared" si="35"/>
+        <f t="shared" si="17"/>
         <v>45950</v>
       </c>
       <c r="J47" s="110">
-        <f t="shared" ref="J47:J49" si="37">I47+1</f>
+        <f t="shared" si="17"/>
         <v>45951</v>
       </c>
       <c r="K47" s="111" t="s">
@@ -9776,12 +9784,11 @@
       <c r="L47" s="110" t="s">
         <v>206</v>
       </c>
-      <c r="M47" s="248"/>
-      <c r="N47" s="248"/>
-      <c r="O47" s="248"/>
-      <c r="P47" s="248"/>
+      <c r="M47" s="200"/>
+      <c r="N47" s="200"/>
+      <c r="O47" s="200"/>
+      <c r="P47" s="200"/>
       <c r="Q47" s="117">
-        <f t="shared" ref="Q47:Q68" si="38">D47*10940</f>
         <v>843222.38</v>
       </c>
       <c r="R47" s="145"/>
@@ -9851,15 +9858,15 @@
         <v>45950</v>
       </c>
       <c r="H48" s="110">
-        <f t="shared" si="33"/>
+        <f t="shared" si="20"/>
         <v>45955</v>
       </c>
       <c r="I48" s="110">
-        <f t="shared" si="35"/>
+        <f t="shared" si="17"/>
         <v>45956</v>
       </c>
       <c r="J48" s="110">
-        <f t="shared" si="37"/>
+        <f t="shared" si="17"/>
         <v>45957</v>
       </c>
       <c r="K48" s="111" t="s">
@@ -9868,12 +9875,11 @@
       <c r="L48" s="110" t="s">
         <v>206</v>
       </c>
-      <c r="M48" s="248"/>
-      <c r="N48" s="248"/>
-      <c r="O48" s="248"/>
-      <c r="P48" s="248"/>
+      <c r="M48" s="200"/>
+      <c r="N48" s="200"/>
+      <c r="O48" s="200"/>
+      <c r="P48" s="200"/>
       <c r="Q48" s="117">
-        <f t="shared" si="38"/>
         <v>395590.39999999997</v>
       </c>
       <c r="R48" s="145"/>
@@ -9943,15 +9949,15 @@
         <v>45956</v>
       </c>
       <c r="H49" s="110">
-        <f t="shared" si="33"/>
+        <f t="shared" si="20"/>
         <v>45961</v>
       </c>
       <c r="I49" s="110">
-        <f t="shared" si="35"/>
+        <f t="shared" si="17"/>
         <v>45962</v>
       </c>
       <c r="J49" s="110">
-        <f t="shared" si="37"/>
+        <f t="shared" si="17"/>
         <v>45963</v>
       </c>
       <c r="K49" s="111" t="s">
@@ -9960,12 +9966,11 @@
       <c r="L49" s="110" t="s">
         <v>206</v>
       </c>
-      <c r="M49" s="248"/>
-      <c r="N49" s="248"/>
-      <c r="O49" s="248"/>
-      <c r="P49" s="248"/>
+      <c r="M49" s="200"/>
+      <c r="N49" s="200"/>
+      <c r="O49" s="200"/>
+      <c r="P49" s="200"/>
       <c r="Q49" s="117">
-        <f t="shared" si="38"/>
         <v>606633.94000000006</v>
       </c>
       <c r="R49" s="145"/>
@@ -10038,7 +10043,7 @@
         <v>45936</v>
       </c>
       <c r="I50" s="110">
-        <f t="shared" ref="I50:I57" si="39">H50+1</f>
+        <f t="shared" si="17"/>
         <v>45937</v>
       </c>
       <c r="J50" s="110">
@@ -10056,7 +10061,6 @@
       <c r="O50" s="138"/>
       <c r="P50" s="138"/>
       <c r="Q50" s="112">
-        <f t="shared" si="38"/>
         <v>395590.39999999997</v>
       </c>
       <c r="R50" s="145"/>
@@ -10122,7 +10126,7 @@
         <v>45936</v>
       </c>
       <c r="G51" s="178">
-        <f t="shared" ref="G51" si="40">H50+1</f>
+        <f t="shared" ref="G51" si="22">H50+1</f>
         <v>45937</v>
       </c>
       <c r="H51" s="178">
@@ -10130,7 +10134,7 @@
         <v>45945</v>
       </c>
       <c r="I51" s="178">
-        <f t="shared" si="39"/>
+        <f t="shared" si="17"/>
         <v>45946</v>
       </c>
       <c r="J51" s="178">
@@ -10148,7 +10152,6 @@
       <c r="O51" s="195"/>
       <c r="P51" s="195"/>
       <c r="Q51" s="193">
-        <f t="shared" si="38"/>
         <v>389485.87999999995</v>
       </c>
       <c r="R51" s="181"/>
@@ -10226,11 +10229,11 @@
         <v>45950</v>
       </c>
       <c r="I52" s="110">
-        <f t="shared" si="39"/>
+        <f t="shared" si="17"/>
         <v>45951</v>
       </c>
       <c r="J52" s="110">
-        <f t="shared" ref="J52:J53" si="41">I52+1</f>
+        <f t="shared" si="17"/>
         <v>45952</v>
       </c>
       <c r="K52" s="110" t="s">
@@ -10239,12 +10242,11 @@
       <c r="L52" s="138" t="s">
         <v>205</v>
       </c>
-      <c r="M52" s="248"/>
-      <c r="N52" s="248"/>
-      <c r="O52" s="248"/>
-      <c r="P52" s="248"/>
+      <c r="M52" s="200"/>
+      <c r="N52" s="200"/>
+      <c r="O52" s="200"/>
+      <c r="P52" s="200"/>
       <c r="Q52" s="117">
-        <f t="shared" si="38"/>
         <v>395590.39999999997</v>
       </c>
       <c r="R52" s="145"/>
@@ -10318,11 +10320,11 @@
         <v>45959</v>
       </c>
       <c r="I53" s="110">
-        <f t="shared" si="39"/>
+        <f t="shared" ref="I53:J68" si="23">H53+1</f>
         <v>45960</v>
       </c>
       <c r="J53" s="110">
-        <f t="shared" si="41"/>
+        <f t="shared" si="23"/>
         <v>45961</v>
       </c>
       <c r="K53" s="110" t="s">
@@ -10331,12 +10333,11 @@
       <c r="L53" s="138" t="s">
         <v>205</v>
       </c>
-      <c r="M53" s="248"/>
-      <c r="N53" s="248"/>
-      <c r="O53" s="248"/>
-      <c r="P53" s="248"/>
+      <c r="M53" s="200"/>
+      <c r="N53" s="200"/>
+      <c r="O53" s="200"/>
+      <c r="P53" s="200"/>
       <c r="Q53" s="117">
-        <f t="shared" si="38"/>
         <v>389485.87999999995</v>
       </c>
       <c r="R53" s="145"/>
@@ -10409,7 +10410,7 @@
         <v>45938</v>
       </c>
       <c r="I54" s="110">
-        <f t="shared" si="39"/>
+        <f t="shared" si="23"/>
         <v>45939</v>
       </c>
       <c r="J54" s="110">
@@ -10422,12 +10423,11 @@
       <c r="L54" s="138" t="s">
         <v>205</v>
       </c>
-      <c r="M54" s="248"/>
-      <c r="N54" s="248"/>
-      <c r="O54" s="248"/>
-      <c r="P54" s="248"/>
+      <c r="M54" s="200"/>
+      <c r="N54" s="200"/>
+      <c r="O54" s="200"/>
+      <c r="P54" s="200"/>
       <c r="Q54" s="117">
-        <f t="shared" si="38"/>
         <v>606633.94000000006</v>
       </c>
       <c r="R54" s="145"/>
@@ -10493,7 +10493,7 @@
         <v>45938</v>
       </c>
       <c r="G55" s="110">
-        <f t="shared" ref="G55" si="42">H54+1</f>
+        <f t="shared" ref="G55" si="24">H54+1</f>
         <v>45939</v>
       </c>
       <c r="H55" s="110">
@@ -10501,7 +10501,7 @@
         <v>45945</v>
       </c>
       <c r="I55" s="110">
-        <f t="shared" si="39"/>
+        <f t="shared" si="23"/>
         <v>45946</v>
       </c>
       <c r="J55" s="110">
@@ -10514,12 +10514,11 @@
       <c r="L55" s="138" t="s">
         <v>205</v>
       </c>
-      <c r="M55" s="248"/>
-      <c r="N55" s="248"/>
-      <c r="O55" s="248"/>
-      <c r="P55" s="248"/>
+      <c r="M55" s="200"/>
+      <c r="N55" s="200"/>
+      <c r="O55" s="200"/>
+      <c r="P55" s="200"/>
       <c r="Q55" s="117">
-        <f t="shared" si="38"/>
         <v>679549.04</v>
       </c>
       <c r="R55" s="145"/>
@@ -10589,15 +10588,15 @@
         <v>45946</v>
       </c>
       <c r="H56" s="110">
-        <f t="shared" ref="H56:H68" si="43">G56+4</f>
+        <f t="shared" ref="H56:H68" si="25">G56+4</f>
         <v>45950</v>
       </c>
       <c r="I56" s="110">
-        <f t="shared" si="39"/>
+        <f t="shared" si="23"/>
         <v>45951</v>
       </c>
       <c r="J56" s="110">
-        <f t="shared" ref="J56:J57" si="44">I56+1</f>
+        <f t="shared" si="23"/>
         <v>45952</v>
       </c>
       <c r="K56" s="110" t="s">
@@ -10606,12 +10605,11 @@
       <c r="L56" s="138" t="s">
         <v>205</v>
       </c>
-      <c r="M56" s="248"/>
-      <c r="N56" s="248"/>
-      <c r="O56" s="248"/>
-      <c r="P56" s="248"/>
+      <c r="M56" s="200"/>
+      <c r="N56" s="200"/>
+      <c r="O56" s="200"/>
+      <c r="P56" s="200"/>
       <c r="Q56" s="117">
-        <f t="shared" si="38"/>
         <v>414965.13999999996</v>
       </c>
       <c r="R56" s="145"/>
@@ -10681,15 +10679,15 @@
         <v>45951</v>
       </c>
       <c r="H57" s="110">
-        <f t="shared" si="43"/>
+        <f t="shared" si="25"/>
         <v>45955</v>
       </c>
       <c r="I57" s="110">
-        <f t="shared" si="39"/>
+        <f t="shared" si="23"/>
         <v>45956</v>
       </c>
       <c r="J57" s="110">
-        <f t="shared" si="44"/>
+        <f t="shared" si="23"/>
         <v>45957</v>
       </c>
       <c r="K57" s="110" t="s">
@@ -10698,12 +10696,11 @@
       <c r="L57" s="138" t="s">
         <v>205</v>
       </c>
-      <c r="M57" s="248"/>
-      <c r="N57" s="248"/>
-      <c r="O57" s="248"/>
-      <c r="P57" s="248"/>
+      <c r="M57" s="200"/>
+      <c r="N57" s="200"/>
+      <c r="O57" s="200"/>
+      <c r="P57" s="200"/>
       <c r="Q57" s="117">
-        <f t="shared" si="38"/>
         <v>395590.39999999997</v>
       </c>
       <c r="R57" s="145"/>
@@ -10773,15 +10770,15 @@
         <v>45956</v>
       </c>
       <c r="H58" s="110">
-        <f t="shared" si="43"/>
+        <f t="shared" si="25"/>
         <v>45960</v>
       </c>
       <c r="I58" s="110">
-        <f t="shared" ref="I58" si="45">H58+1</f>
+        <f t="shared" si="23"/>
         <v>45961</v>
       </c>
       <c r="J58" s="110">
-        <f t="shared" ref="J58" si="46">I58+1</f>
+        <f t="shared" si="23"/>
         <v>45962</v>
       </c>
       <c r="K58" s="110" t="s">
@@ -10790,12 +10787,11 @@
       <c r="L58" s="138" t="s">
         <v>205</v>
       </c>
-      <c r="M58" s="248"/>
-      <c r="N58" s="248"/>
-      <c r="O58" s="248"/>
-      <c r="P58" s="248"/>
+      <c r="M58" s="200"/>
+      <c r="N58" s="200"/>
+      <c r="O58" s="200"/>
+      <c r="P58" s="200"/>
       <c r="Q58" s="117">
-        <f t="shared" si="38"/>
         <v>414965.13999999996</v>
       </c>
       <c r="R58" s="145"/>
@@ -10864,11 +10860,11 @@
         <v>45932</v>
       </c>
       <c r="H59" s="178">
-        <f t="shared" si="43"/>
+        <f t="shared" si="25"/>
         <v>45936</v>
       </c>
       <c r="I59" s="178">
-        <f t="shared" ref="I59:I63" si="47">H59+1</f>
+        <f t="shared" si="23"/>
         <v>45937</v>
       </c>
       <c r="J59" s="178">
@@ -10881,12 +10877,11 @@
       <c r="L59" s="195" t="s">
         <v>205</v>
       </c>
-      <c r="M59" s="249"/>
-      <c r="N59" s="249"/>
-      <c r="O59" s="249"/>
-      <c r="P59" s="249"/>
+      <c r="M59" s="201"/>
+      <c r="N59" s="201"/>
+      <c r="O59" s="201"/>
+      <c r="P59" s="201"/>
       <c r="Q59" s="180">
-        <f t="shared" si="38"/>
         <v>395590.39999999997</v>
       </c>
       <c r="R59" s="181"/>
@@ -10956,15 +10951,15 @@
         <v>45936</v>
       </c>
       <c r="G60" s="110">
-        <f t="shared" ref="G60" si="48">H59+1</f>
+        <f t="shared" ref="G60" si="26">H59+1</f>
         <v>45937</v>
       </c>
       <c r="H60" s="110">
-        <f t="shared" si="43"/>
+        <f t="shared" si="25"/>
         <v>45941</v>
       </c>
       <c r="I60" s="110">
-        <f t="shared" si="47"/>
+        <f t="shared" si="23"/>
         <v>45942</v>
       </c>
       <c r="J60" s="110">
@@ -10977,12 +10972,11 @@
       <c r="L60" s="138" t="s">
         <v>205</v>
       </c>
-      <c r="M60" s="248"/>
-      <c r="N60" s="248"/>
-      <c r="O60" s="248"/>
-      <c r="P60" s="248"/>
+      <c r="M60" s="200"/>
+      <c r="N60" s="200"/>
+      <c r="O60" s="200"/>
+      <c r="P60" s="200"/>
       <c r="Q60" s="117">
-        <f t="shared" si="38"/>
         <v>414965.13999999996</v>
       </c>
       <c r="R60" s="145"/>
@@ -11052,15 +11046,15 @@
         <v>45942</v>
       </c>
       <c r="H61" s="110">
-        <f t="shared" si="43"/>
+        <f t="shared" si="25"/>
         <v>45946</v>
       </c>
       <c r="I61" s="110">
-        <f t="shared" si="47"/>
+        <f t="shared" si="23"/>
         <v>45947</v>
       </c>
       <c r="J61" s="110">
-        <f t="shared" ref="J61:J63" si="49">I61+1</f>
+        <f t="shared" si="23"/>
         <v>45948</v>
       </c>
       <c r="K61" s="110" t="s">
@@ -11069,12 +11063,11 @@
       <c r="L61" s="138" t="s">
         <v>205</v>
       </c>
-      <c r="M61" s="248"/>
-      <c r="N61" s="248"/>
-      <c r="O61" s="248"/>
-      <c r="P61" s="248"/>
+      <c r="M61" s="200"/>
+      <c r="N61" s="200"/>
+      <c r="O61" s="200"/>
+      <c r="P61" s="200"/>
       <c r="Q61" s="117">
-        <f t="shared" si="38"/>
         <v>414965.13999999996</v>
       </c>
       <c r="R61" s="145"/>
@@ -11144,15 +11137,15 @@
         <v>45947</v>
       </c>
       <c r="H62" s="110">
-        <f t="shared" si="43"/>
+        <f t="shared" si="25"/>
         <v>45951</v>
       </c>
       <c r="I62" s="110">
-        <f t="shared" si="47"/>
+        <f t="shared" si="23"/>
         <v>45952</v>
       </c>
       <c r="J62" s="110">
-        <f t="shared" si="49"/>
+        <f t="shared" si="23"/>
         <v>45953</v>
       </c>
       <c r="K62" s="110" t="s">
@@ -11161,12 +11154,11 @@
       <c r="L62" s="138" t="s">
         <v>205</v>
       </c>
-      <c r="M62" s="248"/>
-      <c r="N62" s="248"/>
-      <c r="O62" s="248"/>
-      <c r="P62" s="248"/>
+      <c r="M62" s="200"/>
+      <c r="N62" s="200"/>
+      <c r="O62" s="200"/>
+      <c r="P62" s="200"/>
       <c r="Q62" s="117">
-        <f t="shared" si="38"/>
         <v>479215.76</v>
       </c>
       <c r="R62" s="145"/>
@@ -11236,15 +11228,15 @@
         <v>45952</v>
       </c>
       <c r="H63" s="110">
-        <f t="shared" si="43"/>
+        <f t="shared" si="25"/>
         <v>45956</v>
       </c>
       <c r="I63" s="110">
-        <f t="shared" si="47"/>
+        <f t="shared" si="23"/>
         <v>45957</v>
       </c>
       <c r="J63" s="110">
-        <f t="shared" si="49"/>
+        <f t="shared" si="23"/>
         <v>45958</v>
       </c>
       <c r="K63" s="110" t="s">
@@ -11253,12 +11245,11 @@
       <c r="L63" s="138" t="s">
         <v>205</v>
       </c>
-      <c r="M63" s="248"/>
-      <c r="N63" s="248"/>
-      <c r="O63" s="248"/>
-      <c r="P63" s="248"/>
+      <c r="M63" s="200"/>
+      <c r="N63" s="200"/>
+      <c r="O63" s="200"/>
+      <c r="P63" s="200"/>
       <c r="Q63" s="117">
-        <f t="shared" si="38"/>
         <v>395590.39999999997</v>
       </c>
       <c r="R63" s="145"/>
@@ -11327,11 +11318,11 @@
         <v>45932</v>
       </c>
       <c r="H64" s="110">
-        <f t="shared" si="43"/>
+        <f t="shared" si="25"/>
         <v>45936</v>
       </c>
       <c r="I64" s="110">
-        <f t="shared" ref="I64:I68" si="50">H64+1</f>
+        <f t="shared" si="23"/>
         <v>45937</v>
       </c>
       <c r="J64" s="110">
@@ -11344,12 +11335,11 @@
       <c r="L64" s="138" t="s">
         <v>205</v>
       </c>
-      <c r="M64" s="248"/>
-      <c r="N64" s="248"/>
-      <c r="O64" s="248"/>
-      <c r="P64" s="248"/>
+      <c r="M64" s="200"/>
+      <c r="N64" s="200"/>
+      <c r="O64" s="200"/>
+      <c r="P64" s="200"/>
       <c r="Q64" s="117">
-        <f t="shared" si="38"/>
         <v>395590.39999999997</v>
       </c>
       <c r="R64" s="145"/>
@@ -11415,15 +11405,15 @@
         <v>45936</v>
       </c>
       <c r="G65" s="110">
-        <f t="shared" ref="G65" si="51">H64+1</f>
+        <f t="shared" ref="G65" si="27">H64+1</f>
         <v>45937</v>
       </c>
       <c r="H65" s="110">
-        <f t="shared" si="43"/>
+        <f t="shared" si="25"/>
         <v>45941</v>
       </c>
       <c r="I65" s="110">
-        <f t="shared" si="50"/>
+        <f t="shared" si="23"/>
         <v>45942</v>
       </c>
       <c r="J65" s="110">
@@ -11436,12 +11426,11 @@
       <c r="L65" s="138" t="s">
         <v>205</v>
       </c>
-      <c r="M65" s="248"/>
-      <c r="N65" s="248"/>
-      <c r="O65" s="248"/>
-      <c r="P65" s="248"/>
+      <c r="M65" s="200"/>
+      <c r="N65" s="200"/>
+      <c r="O65" s="200"/>
+      <c r="P65" s="200"/>
       <c r="Q65" s="117">
-        <f t="shared" si="38"/>
         <v>395590.39999999997</v>
       </c>
       <c r="R65" s="145"/>
@@ -11511,15 +11500,15 @@
         <v>45942</v>
       </c>
       <c r="H66" s="110">
-        <f t="shared" si="43"/>
+        <f t="shared" si="25"/>
         <v>45946</v>
       </c>
       <c r="I66" s="110">
-        <f t="shared" si="50"/>
+        <f t="shared" si="23"/>
         <v>45947</v>
       </c>
       <c r="J66" s="110">
-        <f t="shared" ref="J66:J68" si="52">I66+1</f>
+        <f t="shared" si="23"/>
         <v>45948</v>
       </c>
       <c r="K66" s="110" t="s">
@@ -11528,12 +11517,11 @@
       <c r="L66" s="138" t="s">
         <v>205</v>
       </c>
-      <c r="M66" s="248"/>
-      <c r="N66" s="248"/>
-      <c r="O66" s="248"/>
-      <c r="P66" s="248"/>
+      <c r="M66" s="200"/>
+      <c r="N66" s="200"/>
+      <c r="O66" s="200"/>
+      <c r="P66" s="200"/>
       <c r="Q66" s="117">
-        <f t="shared" si="38"/>
         <v>395590.39999999997</v>
       </c>
       <c r="R66" s="145"/>
@@ -11603,15 +11591,15 @@
         <v>45947</v>
       </c>
       <c r="H67" s="178">
-        <f t="shared" si="43"/>
+        <f t="shared" si="25"/>
         <v>45951</v>
       </c>
       <c r="I67" s="178">
-        <f t="shared" si="50"/>
+        <f t="shared" si="23"/>
         <v>45952</v>
       </c>
       <c r="J67" s="178">
-        <f t="shared" si="52"/>
+        <f t="shared" si="23"/>
         <v>45953</v>
       </c>
       <c r="K67" s="178" t="s">
@@ -11620,12 +11608,11 @@
       <c r="L67" s="195" t="s">
         <v>205</v>
       </c>
-      <c r="M67" s="249"/>
-      <c r="N67" s="249"/>
-      <c r="O67" s="249"/>
-      <c r="P67" s="249"/>
+      <c r="M67" s="201"/>
+      <c r="N67" s="201"/>
+      <c r="O67" s="201"/>
+      <c r="P67" s="201"/>
       <c r="Q67" s="180">
-        <f t="shared" si="38"/>
         <v>395590.39999999997</v>
       </c>
       <c r="R67" s="181"/>
@@ -11699,15 +11686,15 @@
         <v>45952</v>
       </c>
       <c r="H68" s="110">
-        <f t="shared" si="43"/>
+        <f t="shared" si="25"/>
         <v>45956</v>
       </c>
       <c r="I68" s="110">
-        <f t="shared" si="50"/>
+        <f t="shared" si="23"/>
         <v>45957</v>
       </c>
       <c r="J68" s="110">
-        <f t="shared" si="52"/>
+        <f t="shared" si="23"/>
         <v>45958</v>
       </c>
       <c r="K68" s="110" t="s">
@@ -11716,12 +11703,11 @@
       <c r="L68" s="138" t="s">
         <v>205</v>
       </c>
-      <c r="M68" s="248"/>
-      <c r="N68" s="248"/>
-      <c r="O68" s="248"/>
-      <c r="P68" s="248"/>
+      <c r="M68" s="200"/>
+      <c r="N68" s="200"/>
+      <c r="O68" s="200"/>
+      <c r="P68" s="200"/>
       <c r="Q68" s="117">
-        <f t="shared" si="38"/>
         <v>395590.39999999997</v>
       </c>
       <c r="R68" s="145"/>
@@ -11794,56 +11780,56 @@
       <c r="S69" s="155"/>
       <c r="T69" s="84"/>
       <c r="U69" s="151">
-        <f t="shared" ref="U69:Z69" si="53">SUM(U21:U68)</f>
+        <f t="shared" ref="U69:Z69" si="28">SUM(U21:U68)</f>
         <v>4</v>
       </c>
       <c r="V69" s="151">
-        <f t="shared" si="53"/>
+        <f t="shared" si="28"/>
         <v>1</v>
       </c>
       <c r="W69" s="151">
-        <f t="shared" si="53"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="X69" s="151">
-        <f t="shared" si="53"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="Y69" s="151">
-        <f t="shared" si="53"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="Z69" s="151">
-        <f t="shared" si="53"/>
+        <f t="shared" si="28"/>
         <v>5</v>
       </c>
       <c r="AA69" s="152"/>
       <c r="AB69" s="106">
-        <f t="shared" ref="AB69:AH69" si="54">SUM(AB21:AB68)</f>
+        <f t="shared" ref="AB69:AH69" si="29">SUM(AB21:AB68)</f>
         <v>2420223.38</v>
       </c>
       <c r="AC69" s="106">
-        <f t="shared" si="54"/>
+        <f t="shared" si="29"/>
         <v>395590.39999999997</v>
       </c>
       <c r="AD69" s="106">
-        <f t="shared" si="54"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="AE69" s="106">
-        <f t="shared" si="54"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="AF69" s="106">
-        <f t="shared" si="54"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="AG69" s="106">
-        <f t="shared" si="54"/>
+        <f t="shared" si="29"/>
         <v>2815813.78</v>
       </c>
       <c r="AH69" s="92">
-        <f t="shared" si="54"/>
+        <f t="shared" si="29"/>
         <v>24750437.199999996</v>
       </c>
     </row>
@@ -11862,6 +11848,7 @@
   </sheetData>
   <autoFilter ref="A20:AH69" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <mergeCells count="17">
+    <mergeCell ref="U18:Z18"/>
     <mergeCell ref="F18:J18"/>
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="AH18:AH19"/>
@@ -11878,20 +11865,19 @@
     <mergeCell ref="Y19:Y20"/>
     <mergeCell ref="Q18:Q19"/>
     <mergeCell ref="S18:S19"/>
-    <mergeCell ref="U18:Z18"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B1:B2">
-    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
-    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52:B58 B21:B26 B28 B30:B50">
-    <cfRule type="duplicateValues" dxfId="2" priority="13140"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="13141"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="13142"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>